<commit_message>
Tile template and additional csv support
Finalized tile template for alpha and add full level loading support
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BoardGraphics" sheetId="6" r:id="rId1"/>
-    <sheet name="BoardContents" sheetId="3" r:id="rId2"/>
-    <sheet name="BoardTriggers" sheetId="4" r:id="rId3"/>
+    <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
+    <sheet name="TileTriggers" sheetId="4" r:id="rId2"/>
+    <sheet name="TileContents" sheetId="3" r:id="rId3"/>
     <sheet name="BoardEnums" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="contentEnums">BoardEnums!$B$2:$B$35</definedName>
-    <definedName name="graphicEnums">BoardEnums!$A$2:$A$36</definedName>
+    <definedName name="contentEnums">BoardEnums!$B$2:$B$5</definedName>
+    <definedName name="frameIndexEnums">BoardEnums!$D$2:$D$48</definedName>
+    <definedName name="graphicEnums">BoardEnums!$A$2:$A$5</definedName>
     <definedName name="triggerEnums">BoardEnums!$C$2:$C$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="68">
   <si>
     <t>forestGrass</t>
   </si>
@@ -71,19 +72,189 @@
   </si>
   <si>
     <t>separate with |</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>UP_LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT</t>
+  </si>
+  <si>
+    <t>RIGHT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_DOWN</t>
+  </si>
+  <si>
+    <t>RIGHT_DOWN-RIGHT_DOWN</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>RIGHT_DOWN</t>
+  </si>
+  <si>
+    <t>UP-RIGHT</t>
+  </si>
+  <si>
+    <t>DOWN-RIGHT</t>
+  </si>
+  <si>
+    <t>DOWN-LEFT</t>
+  </si>
+  <si>
+    <t>UP-LEFT</t>
+  </si>
+  <si>
+    <t>DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>RIGHT_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>UP_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_DOWN_DOWN-LEFT_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>Frame Direction Priority Order</t>
+  </si>
+  <si>
+    <t>(Number of directions)</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>RIGHT_DOWN-RIGHT_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN-RIGHT_DOWN</t>
+  </si>
+  <si>
+    <t>RIGHT_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>RIGHT_DOWN-RIGHT_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>UP_DOWN_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN_DOWN-LEFT_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN-RIGHT_DOWN</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN-RIGHT_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN-RIGHT_DOWN_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN-RIGHT_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_RIGHT_DOWN-RIGHT_DOWN_DOWN-LEFT_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN_DOWN-LEFT_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN-RIGHT_DOWN_LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN-RIGHT_DOWN_LEFT_UP-LEFT</t>
+  </si>
+  <si>
+    <t>UP_UP-RIGHT_RIGHT_DOWN-RIGHT_DOWN_DOWN-LEFT_LEFT</t>
+  </si>
+  <si>
+    <t>Frame Index Enums (TileFrameIndices)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,9 +292,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,8 +1154,578 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:P11">
+      <formula1>triggerEnums</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,11 +1735,11 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1035,7 +1780,7 @@
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1490,7 +2235,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -1535,7 +2280,7 @@
         <v>9</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1548,590 +2293,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:P11">
-      <formula1>triggerEnums</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2141,30 +2323,49 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2174,16 +2375,280 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="B2:B3">
+    <sortCondition ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed map loading and added full support for forest maps
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
@@ -20,8 +20,8 @@
   <definedNames>
     <definedName name="contentEnums">BoardEnums!$B$2:$B$5</definedName>
     <definedName name="frameIndexEnums">BoardEnums!$D$2:$D$48</definedName>
-    <definedName name="graphicEnums">BoardEnums!$A$2:$A$5</definedName>
-    <definedName name="triggerEnums">BoardEnums!$C$2:$C$4</definedName>
+    <definedName name="graphicEnums">BoardEnums!$A$2:$A$10</definedName>
+    <definedName name="triggerEnums">BoardEnums!$C$2:$C$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,19 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="68">
-  <si>
-    <t>forestGrass</t>
-  </si>
-  <si>
-    <t>forestTree</t>
-  </si>
-  <si>
-    <t>forestGroundPebble</t>
-  </si>
-  <si>
-    <t>forestDirt</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="74">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -237,6 +225,36 @@
   </si>
   <si>
     <t>Frame Index Enums (TileFrameIndices)</t>
+  </si>
+  <si>
+    <t>forest_Dirt</t>
+  </si>
+  <si>
+    <t>forest_GrassPath</t>
+  </si>
+  <si>
+    <t>forest_DirtPath</t>
+  </si>
+  <si>
+    <t>forest_DirtTree</t>
+  </si>
+  <si>
+    <t>forest_GrassTree</t>
+  </si>
+  <si>
+    <t>forest_Grass</t>
+  </si>
+  <si>
+    <t>forest_DirtyGrass</t>
+  </si>
+  <si>
+    <t>permanent</t>
+  </si>
+  <si>
+    <t>forest_DungeonEntrance</t>
+  </si>
+  <si>
+    <t>forest_PlayerStart</t>
   </si>
 </sst>
 </file>
@@ -581,563 +599,563 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="16" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1154,560 +1172,560 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +1743,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+      <selection sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,552 +1753,552 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2298,12 +2316,12 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.140625" bestFit="1" customWidth="1"/>
@@ -2315,333 +2333,351 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
       <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
         <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forest tile sprites added. Export script now support exporting multiple times
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -18,10 +18,10 @@
     <sheet name="BoardEnums" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="contentEnums">BoardEnums!$B$2:$B$5</definedName>
+    <definedName name="contentEnums">BoardEnums!$B$2:$B$6</definedName>
     <definedName name="frameIndexEnums">BoardEnums!$D$2:$D$48</definedName>
-    <definedName name="graphicEnums">BoardEnums!$A$2:$A$10</definedName>
-    <definedName name="triggerEnums">BoardEnums!$C$2:$C$5</definedName>
+    <definedName name="graphicEnums">BoardEnums!$A$2:$A$11</definedName>
+    <definedName name="triggerEnums">BoardEnums!$C$2:$C$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="75">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -251,10 +251,13 @@
     <t>permanent</t>
   </si>
   <si>
-    <t>forest_DungeonEntrance</t>
-  </si>
-  <si>
     <t>forest_PlayerStart</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>forest_Exit</t>
   </si>
 </sst>
 </file>
@@ -600,562 +603,563 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:P11"/>
+      <selection activeCell="B2" sqref="B2:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1173,10 +1177,13 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P11"/>
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1233,46 +1240,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>5</v>
@@ -1283,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -1322,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>5</v>
@@ -1333,7 +1340,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -1372,7 +1379,7 @@
         <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>5</v>
@@ -1383,7 +1390,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -1422,7 +1429,7 @@
         <v>5</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>5</v>
@@ -1433,7 +1440,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -1472,7 +1479,7 @@
         <v>5</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>5</v>
@@ -1483,7 +1490,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -1522,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>5</v>
@@ -1533,7 +1540,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1572,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>5</v>
@@ -1583,7 +1590,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1622,7 +1629,7 @@
         <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>5</v>
@@ -1633,7 +1640,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1672,7 +1679,7 @@
         <v>5</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>5</v>
@@ -1748,7 +1755,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -2316,7 +2323,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2416,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -2423,6 +2430,9 @@
       <c r="A6" t="s">
         <v>68</v>
       </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
@@ -2456,7 +2466,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -2468,7 +2478,7 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added beginning to movement support.
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -603,7 +603,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +926,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Modified game loading to include entitiies
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -15,13 +15,15 @@
     <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
     <sheet name="TileTriggers" sheetId="4" r:id="rId2"/>
     <sheet name="TileContents" sheetId="3" r:id="rId3"/>
-    <sheet name="BoardEnums" sheetId="2" r:id="rId4"/>
+    <sheet name="TileEntities" sheetId="7" r:id="rId4"/>
+    <sheet name="BoardEnums" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="contentEnums">BoardEnums!$B$2:$B$6</definedName>
+    <definedName name="contentEnums">BoardEnums!$B$2:$B$11</definedName>
+    <definedName name="entityEnums">BoardEnums!$E$2:$E$5</definedName>
     <definedName name="frameIndexEnums">BoardEnums!$D$2:$D$48</definedName>
-    <definedName name="graphicEnums">BoardEnums!$A$2:$A$11</definedName>
-    <definedName name="triggerEnums">BoardEnums!$C$2:$C$7</definedName>
+    <definedName name="graphicEnums">BoardEnums!$A$2:$A$10</definedName>
+    <definedName name="triggerEnums">BoardEnums!$C$2:$C$6</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="77">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -251,13 +253,19 @@
     <t>permanent</t>
   </si>
   <si>
-    <t>forest_PlayerStart</t>
-  </si>
-  <si>
     <t>hidden</t>
   </si>
   <si>
     <t>forest_Exit</t>
+  </si>
+  <si>
+    <t>Entity Enums</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>wisp</t>
   </si>
 </sst>
 </file>
@@ -603,242 +611,241 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="P11" sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="19.28515625" customWidth="1"/>
+    <col min="1" max="16" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>66</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>66</v>
@@ -859,48 +866,48 @@
         <v>66</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>66</v>
@@ -909,48 +916,48 @@
         <v>66</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>66</v>
@@ -959,48 +966,48 @@
         <v>66</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>66</v>
@@ -1009,62 +1016,62 @@
         <v>66</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>66</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>66</v>
@@ -1106,60 +1113,60 @@
         <v>66</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1177,12 +1184,12 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B10"/>
+      <selection activeCell="A14" sqref="A14:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="16" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1240,46 +1247,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>5</v>
@@ -1290,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
@@ -1329,7 +1336,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>5</v>
@@ -1346,7 +1353,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
@@ -1379,7 +1386,7 @@
         <v>5</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>5</v>
@@ -1417,7 +1424,7 @@
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>5</v>
@@ -1429,7 +1436,7 @@
         <v>5</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>5</v>
@@ -1443,7 +1450,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -1455,7 +1462,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>5</v>
@@ -1464,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
@@ -1479,7 +1486,7 @@
         <v>5</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>5</v>
@@ -1508,7 +1515,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>5</v>
@@ -1529,7 +1536,7 @@
         <v>5</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>5</v>
@@ -1579,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>5</v>
@@ -1629,7 +1636,7 @@
         <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>5</v>
@@ -1640,7 +1647,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1679,7 +1686,7 @@
         <v>5</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>5</v>
@@ -1750,12 +1757,13 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P11"/>
+      <selection activeCell="P23" sqref="A13:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -2320,10 +2328,580 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:P11">
+      <formula1>entityEnums</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,6 +2910,7 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" customWidth="1"/>
@@ -2351,10 +2930,12 @@
       <c r="D1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2369,7 +2950,10 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2386,7 +2970,10 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2403,10 +2990,12 @@
       <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2416,15 +3005,14 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2436,10 +3024,9 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2448,7 +3035,7 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2459,34 +3046,28 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
       <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" t="s">

</xml_diff>

<commit_message>
Fixed level 0 map to not have a trap on a tree
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
@@ -610,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="P11" sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:P24"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,22 +1515,22 @@
         <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="L7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>5</v>
@@ -1577,7 +1577,7 @@
         <v>5</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>5</v>
@@ -1624,13 +1624,13 @@
         <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Add item display and effect support
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="78">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>wisp</t>
+  </si>
+  <si>
+    <t>bones</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P11" sqref="A1:P11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7:N9"/>
     </sheetView>
   </sheetViews>
@@ -1757,7 +1760,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="A13:P23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,10 +1830,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -2330,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Add item display and effect support"
This reverts commit 7cb43a7698ae69bddca5cd0c1e46b3f452ccb0f3.
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="77">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>wisp</t>
-  </si>
-  <si>
-    <t>bones</t>
   </si>
 </sst>
 </file>
@@ -614,7 +611,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P11" sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7:N9"/>
     </sheetView>
   </sheetViews>
@@ -1760,7 +1757,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="P23" sqref="A13:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,10 +1827,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -2333,8 +2330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Revert "Add item display and effect support""
This reverts commit b0834b0fc9b70f2ca4b3c415fb4a1b061bb35288.
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TileGraphics" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="78">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>wisp</t>
+  </si>
+  <si>
+    <t>bones</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P11" sqref="A1:P11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7:N9"/>
     </sheetView>
   </sheetViews>
@@ -1757,7 +1760,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="A13:P23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,10 +1830,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -2330,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated level 1 to have more things
</commit_message>
<xml_diff>
--- a/level0.xlsx
+++ b/level0.xlsx
@@ -614,7 +614,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P11" sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,8 +1759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>5</v>
@@ -1951,10 +1951,10 @@
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>5</v>
@@ -2086,7 +2086,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>5</v>
@@ -2095,10 +2095,10 @@
         <v>5</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>5</v>
@@ -2127,28 +2127,28 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>5</v>
@@ -2192,7 +2192,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>5</v>
@@ -2204,7 +2204,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>5</v>
@@ -2333,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>5</v>
@@ -2577,7 +2577,7 @@
         <v>5</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>5</v>
@@ -2650,7 +2650,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
@@ -2733,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>5</v>

</xml_diff>